<commit_message>
Firmware complete and ready for testing
</commit_message>
<xml_diff>
--- a/DMH_VCO_40106_Firmware/Note_Frequencies.xlsx
+++ b/DMH_VCO_40106_Firmware/Note_Frequencies.xlsx
@@ -1,44 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\DMH-VCO-40106\DMH_VCO_40106_Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\GitHub\DMH-VCO-40106\DMH_VCO_40106_Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD87CBA8-1A22-43CE-9925-88B7D8F997C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB350B8E-F900-4F7A-81EC-B6A31501B4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA574870-E15A-422E-A7FA-740D62337FD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{DA574870-E15A-422E-A7FA-740D62337FD4}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
     <sheet name="uint16" sheetId="2" r:id="rId2"/>
     <sheet name="float" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>C0</t>
   </si>
@@ -362,6 +351,9 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>B8</t>
   </si>
 </sst>
 </file>
@@ -766,20 +758,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D25FA8-86E1-434D-9EE0-CE736711B434}">
-  <dimension ref="C2:N101"/>
+  <dimension ref="C2:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L102" sqref="L102:M102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="8" max="14" width="10.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="8" max="14" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>106</v>
       </c>
@@ -799,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="I3" s="3">
         <v>0.5</v>
       </c>
@@ -814,7 +806,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F4" s="1" t="s">
         <v>107</v>
       </c>
@@ -843,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -882,7 +874,7 @@
         <v>16.83775537297268</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1.0594631000000001</v>
       </c>
@@ -921,7 +913,7 @@
         <v>17.838980504491296</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F7" s="1">
         <v>2</v>
       </c>
@@ -957,7 +949,7 @@
         <v>18.899741586127917</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
         <v>3</v>
       </c>
@@ -993,7 +985,7 @@
         <v>20.023578810038</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F9" s="1">
         <v>4</v>
       </c>
@@ -1029,7 +1021,7 @@
         <v>21.214242879177171</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F10" s="1">
         <v>5</v>
       </c>
@@ -1065,7 +1057,7 @@
         <v>22.475707524925973</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F11" s="1">
         <v>6</v>
       </c>
@@ -1101,7 +1093,7 @@
         <v>23.812182769051404</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <v>7</v>
       </c>
@@ -1137,7 +1129,7 @@
         <v>25.228128974265786</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F13" s="1">
         <v>8</v>
       </c>
@@ -1173,7 +1165,7 @@
         <v>26.728271730275456</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F14" s="1">
         <v>9</v>
       </c>
@@ -1208,7 +1200,7 @@
         <v>28.317617625000004</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F15" s="1">
         <v>10</v>
       </c>
@@ -1244,7 +1236,7 @@
         <v>30.001470953597142</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F16" s="1">
         <v>11</v>
       </c>
@@ -1280,7 +1272,7 @@
         <v>31.785451421057989</v>
       </c>
     </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="1">
         <v>12</v>
       </c>
@@ -1316,7 +1308,7 @@
         <v>33.675512897453501</v>
       </c>
     </row>
-    <row r="18" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F18" s="1">
         <v>13</v>
       </c>
@@ -1352,7 +1344,7 @@
         <v>35.677963288426078</v>
       </c>
     </row>
-    <row r="19" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F19" s="1">
         <v>14</v>
       </c>
@@ -1388,7 +1380,7 @@
         <v>37.799485587242089</v>
       </c>
     </row>
-    <row r="20" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F20" s="1">
         <v>15</v>
       </c>
@@ -1424,7 +1416,7 @@
         <v>40.047160178664832</v>
       </c>
     </row>
-    <row r="21" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F21" s="1">
         <v>16</v>
       </c>
@@ -1460,7 +1452,7 @@
         <v>42.428488469084797</v>
       </c>
     </row>
-    <row r="22" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F22" s="1">
         <v>17</v>
       </c>
@@ -1496,7 +1488,7 @@
         <v>44.95141792177084</v>
       </c>
     </row>
-    <row r="23" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F23" s="1">
         <v>18</v>
       </c>
@@ -1532,7 +1524,7 @@
         <v>47.624368580794894</v>
       </c>
     </row>
-    <row r="24" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F24" s="1">
         <v>19</v>
       </c>
@@ -1568,7 +1560,7 @@
         <v>50.456261172151571</v>
       </c>
     </row>
-    <row r="25" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F25" s="1">
         <v>20</v>
       </c>
@@ -1604,7 +1596,7 @@
         <v>53.456546875857342</v>
       </c>
     </row>
-    <row r="26" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F26" s="1">
         <v>21</v>
       </c>
@@ -1640,7 +1632,7 @@
         <v>56.635238868391141</v>
       </c>
     </row>
-    <row r="27" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F27" s="1">
         <v>22</v>
       </c>
@@ -1676,7 +1668,7 @@
         <v>60.002945740746171</v>
       </c>
     </row>
-    <row r="28" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F28" s="1">
         <v>23</v>
       </c>
@@ -1712,7 +1704,7 @@
         <v>63.570906903622742</v>
       </c>
     </row>
-    <row r="29" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F29" s="1">
         <v>24</v>
       </c>
@@ -1748,7 +1740,7 @@
         <v>67.351030097923555</v>
       </c>
     </row>
-    <row r="30" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F30" s="1">
         <v>25</v>
       </c>
@@ -1784,7 +1776,7 @@
         <v>71.355931135739411</v>
       </c>
     </row>
-    <row r="31" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F31" s="1">
         <v>26</v>
       </c>
@@ -1820,7 +1812,7 @@
         <v>75.598976004457</v>
       </c>
     </row>
-    <row r="32" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F32" s="1">
         <v>27</v>
       </c>
@@ -1856,7 +1848,7 @@
         <v>80.094325474507627</v>
       </c>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" s="1">
         <v>28</v>
       </c>
@@ -1892,7 +1884,7 @@
         <v>84.856982359630834</v>
       </c>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" s="1">
         <v>29</v>
       </c>
@@ -1928,7 +1920,7 @@
         <v>89.902841587379811</v>
       </c>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F35" s="1">
         <v>30</v>
       </c>
@@ -1964,7 +1956,7 @@
         <v>95.248743246974328</v>
       </c>
     </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F36" s="1">
         <v>31</v>
       </c>
@@ -2000,7 +1992,7 @@
         <v>100.91252879154351</v>
       </c>
     </row>
-    <row r="37" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F37" s="1">
         <v>32</v>
       </c>
@@ -2036,7 +2028,7 @@
         <v>106.91310058232794</v>
       </c>
     </row>
-    <row r="38" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F38" s="1">
         <v>33</v>
       </c>
@@ -2072,7 +2064,7 @@
         <v>113.27048497356498</v>
       </c>
     </row>
-    <row r="39" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F39" s="1">
         <v>34</v>
       </c>
@@ -2108,7 +2100,7 @@
         <v>120.0058991485966</v>
       </c>
     </row>
-    <row r="40" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F40" s="1">
         <v>35</v>
       </c>
@@ -2144,7 +2136,7 @@
         <v>127.14182193025952</v>
       </c>
     </row>
-    <row r="41" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F41" s="1">
         <v>36</v>
       </c>
@@ -2180,7 +2172,7 @@
         <v>134.70206880188076</v>
       </c>
     </row>
-    <row r="42" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F42" s="1">
         <v>37</v>
       </c>
@@ -2216,7 +2208,7 @@
         <v>142.71187138925387</v>
       </c>
     </row>
-    <row r="43" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F43" s="1">
         <v>38</v>
       </c>
@@ -2252,7 +2244,7 @@
         <v>151.19796166886024</v>
       </c>
     </row>
-    <row r="44" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F44" s="1">
         <v>39</v>
       </c>
@@ -2288,7 +2280,7 @@
         <v>160.18866118337186</v>
       </c>
     </row>
-    <row r="45" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F45" s="1">
         <v>40</v>
       </c>
@@ -2324,7 +2316,7 @@
         <v>169.71397556218483</v>
       </c>
     </row>
-    <row r="46" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F46" s="1">
         <v>41</v>
       </c>
@@ -2360,7 +2352,7 @@
         <v>179.80569466243662</v>
       </c>
     </row>
-    <row r="47" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F47" s="1">
         <v>42</v>
       </c>
@@ -2396,7 +2388,7 @@
         <v>190.49749866471853</v>
       </c>
     </row>
-    <row r="48" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F48" s="1">
         <v>43</v>
       </c>
@@ -2432,7 +2424,7 @@
         <v>201.8250704775686</v>
       </c>
     </row>
-    <row r="49" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F49" s="1">
         <v>44</v>
       </c>
@@ -2468,7 +2460,7 @@
         <v>213.82621482588331</v>
       </c>
     </row>
-    <row r="50" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F50" s="1">
         <v>45</v>
       </c>
@@ -2504,7 +2496,7 @@
         <v>226.5409844206963</v>
       </c>
     </row>
-    <row r="51" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F51" s="1">
         <v>46</v>
       </c>
@@ -2540,7 +2532,7 @@
         <v>240.01181363140267</v>
       </c>
     </row>
-    <row r="52" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F52" s="1">
         <v>47</v>
       </c>
@@ -2576,7 +2568,7 @@
         <v>254.28366010654815</v>
       </c>
     </row>
-    <row r="53" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F53" s="1">
         <v>48</v>
       </c>
@@ -2612,7 +2604,7 @@
         <v>269.40415481582988</v>
       </c>
     </row>
-    <row r="54" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F54" s="1">
         <v>49</v>
       </c>
@@ -2648,7 +2640,7 @@
         <v>285.42376101405904</v>
       </c>
     </row>
-    <row r="55" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F55" s="1">
         <v>50</v>
       </c>
@@ -2684,7 +2676,7 @@
         <v>302.39594265761417</v>
       </c>
     </row>
-    <row r="56" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F56" s="1">
         <v>51</v>
       </c>
@@ -2720,7 +2712,7 @@
         <v>320.37734283545819</v>
       </c>
     </row>
-    <row r="57" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F57" s="1">
         <v>52</v>
       </c>
@@ -2756,7 +2748,7 @@
         <v>339.4279728102174</v>
       </c>
     </row>
-    <row r="58" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F58" s="1">
         <v>53</v>
       </c>
@@ -2792,7 +2784,7 @@
         <v>359.61141230022861</v>
       </c>
     </row>
-    <row r="59" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F59" s="1">
         <v>54</v>
       </c>
@@ -2828,7 +2820,7 @@
         <v>380.99502167097842</v>
       </c>
     </row>
-    <row r="60" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F60" s="1">
         <v>55</v>
       </c>
@@ -2864,7 +2856,7 @@
         <v>403.65016674410197</v>
       </c>
     </row>
-    <row r="61" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F61" s="1">
         <v>56</v>
       </c>
@@ -2900,7 +2892,7 @@
         <v>427.65245697422324</v>
       </c>
     </row>
-    <row r="62" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F62" s="1">
         <v>57</v>
       </c>
@@ -2936,7 +2928,7 @@
         <v>453.08199778852725</v>
       </c>
     </row>
-    <row r="63" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F63" s="1">
         <v>58</v>
       </c>
@@ -2972,7 +2964,7 @@
         <v>480.02365793122624</v>
       </c>
     </row>
-    <row r="64" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F64" s="1">
         <v>59</v>
       </c>
@@ -3008,7 +3000,7 @@
         <v>508.56735270515662</v>
       </c>
     </row>
-    <row r="65" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F65" s="1">
         <v>60</v>
       </c>
@@ -3044,7 +3036,7 @@
         <v>538.80834405579867</v>
       </c>
     </row>
-    <row r="66" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F66" s="1">
         <v>61</v>
       </c>
@@ -3080,7 +3072,7 @@
         <v>570.84755849922317</v>
       </c>
     </row>
-    <row r="67" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F67" s="1">
         <v>62</v>
       </c>
@@ -3116,7 +3108,7 @@
         <v>604.79192395501832</v>
       </c>
     </row>
-    <row r="68" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F68" s="1">
         <v>63</v>
       </c>
@@ -3152,7 +3144,7 @@
         <v>640.75472660834794</v>
       </c>
     </row>
-    <row r="69" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F69" s="1">
         <v>64</v>
       </c>
@@ -3188,7 +3180,7 @@
         <v>678.85598899213289</v>
       </c>
     </row>
-    <row r="70" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F70" s="1">
         <v>65</v>
       </c>
@@ -3224,7 +3216,7 @@
         <v>719.22287055117113</v>
       </c>
     </row>
-    <row r="71" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F71" s="1">
         <v>66</v>
       </c>
@@ -3260,7 +3252,7 @@
         <v>761.99009202504249</v>
       </c>
     </row>
-    <row r="72" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F72" s="1">
         <v>67</v>
       </c>
@@ -3296,7 +3288,7 @@
         <v>807.30038506613687</v>
       </c>
     </row>
-    <row r="73" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F73" s="1">
         <v>68</v>
       </c>
@@ -3332,7 +3324,7 @@
         <v>855.30496859336313</v>
       </c>
     </row>
-    <row r="74" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F74" s="1">
         <v>69</v>
       </c>
@@ -3368,7 +3360,7 @@
         <v>906.16405347132729</v>
       </c>
     </row>
-    <row r="75" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F75" s="1">
         <v>70</v>
       </c>
@@ -3404,7 +3396,7 @@
         <v>960.04737719929824</v>
       </c>
     </row>
-    <row r="76" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F76" s="1">
         <v>71</v>
       </c>
@@ -3440,7 +3432,7 @@
         <v>1017.1347703944379</v>
       </c>
     </row>
-    <row r="77" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F77" s="1">
         <v>72</v>
       </c>
@@ -3476,7 +3468,7 @@
         <v>1077.6167569598792</v>
       </c>
     </row>
-    <row r="78" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F78" s="1">
         <v>73</v>
       </c>
@@ -3512,7 +3504,7 @@
         <v>1141.6951899406604</v>
       </c>
     </row>
-    <row r="79" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F79" s="1">
         <v>74</v>
       </c>
@@ -3548,7 +3540,7 @@
         <v>1209.5839251896209</v>
       </c>
     </row>
-    <row r="80" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F80" s="1">
         <v>75</v>
       </c>
@@ -3584,7 +3576,7 @@
         <v>1281.509535091564</v>
       </c>
     </row>
-    <row r="81" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F81" s="1">
         <v>76</v>
       </c>
@@ -3604,7 +3596,7 @@
         <v>1314.8105816956488</v>
       </c>
       <c r="K81" s="4">
-        <f t="shared" ref="K81:K101" si="14">K80*$C$6</f>
+        <f t="shared" ref="K81:K102" si="14">K80*$C$6</f>
         <v>1318.5106979849916</v>
       </c>
       <c r="L81" s="4">
@@ -3620,7 +3612,7 @@
         <v>1357.7120647276674</v>
       </c>
     </row>
-    <row r="82" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F82" s="1">
         <v>77</v>
       </c>
@@ -3652,11 +3644,11 @@
         <v>1417.6796322370592</v>
       </c>
       <c r="N82" s="4">
-        <f t="shared" ref="N82:N100" si="18">AVERAGE(K82,K83)</f>
+        <f t="shared" ref="N82:N101" si="18">AVERAGE(K82,K83)</f>
         <v>1438.4458330037751</v>
       </c>
     </row>
-    <row r="83" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F83" s="1">
         <v>78</v>
       </c>
@@ -3692,7 +3684,7 @@
         <v>1523.9802814162622</v>
       </c>
     </row>
-    <row r="84" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F84" s="1">
         <v>79</v>
       </c>
@@ -3728,7 +3720,7 @@
         <v>1614.6008732881455</v>
       </c>
     </row>
-    <row r="85" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F85" s="1">
         <v>80</v>
       </c>
@@ -3764,7 +3756,7 @@
         <v>1710.6100464765659</v>
       </c>
     </row>
-    <row r="86" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F86" s="1">
         <v>81</v>
       </c>
@@ -3800,7 +3792,7 @@
         <v>1812.328222731207</v>
       </c>
     </row>
-    <row r="87" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F87" s="1">
         <v>82</v>
       </c>
@@ -3836,7 +3828,7 @@
         <v>1920.094877072295</v>
       </c>
     </row>
-    <row r="88" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F88" s="1">
         <v>83</v>
       </c>
@@ -3872,7 +3864,7 @@
         <v>2034.2696707571326</v>
       </c>
     </row>
-    <row r="89" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F89" s="1">
         <v>84</v>
       </c>
@@ -3908,7 +3900,7 @@
         <v>2155.2336516163314</v>
       </c>
     </row>
-    <row r="90" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F90" s="1">
         <v>85</v>
       </c>
@@ -3944,7 +3936,7 @@
         <v>2283.3905257657589</v>
       </c>
     </row>
-    <row r="91" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F91" s="1">
         <v>86</v>
       </c>
@@ -3980,7 +3972,7 @@
         <v>2419.1680049384204</v>
       </c>
     </row>
-    <row r="92" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F92" s="1">
         <v>87</v>
       </c>
@@ -4016,7 +4008,7 @@
         <v>2563.0192339328746</v>
       </c>
     </row>
-    <row r="93" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F93" s="1">
         <v>88</v>
       </c>
@@ -4052,7 +4044,7 @@
         <v>2715.4243029421486</v>
       </c>
     </row>
-    <row r="94" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F94" s="1">
         <v>89</v>
       </c>
@@ -4088,7 +4080,7 @@
         <v>2876.8918498104285</v>
       </c>
     </row>
-    <row r="95" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F95" s="1">
         <v>90</v>
       </c>
@@ -4124,7 +4116,7 @@
         <v>3047.9607575648915</v>
       </c>
     </row>
-    <row r="96" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F96" s="1">
         <v>91</v>
       </c>
@@ -4160,7 +4152,7 @@
         <v>3229.2019528880483</v>
       </c>
     </row>
-    <row r="97" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F97" s="1">
         <v>92</v>
       </c>
@@ -4196,7 +4188,7 @@
         <v>3421.2203115328261</v>
       </c>
     </row>
-    <row r="98" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F98" s="1">
         <v>93</v>
       </c>
@@ -4232,7 +4224,7 @@
         <v>3624.6566770395339</v>
       </c>
     </row>
-    <row r="99" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F99" s="1">
         <v>94</v>
       </c>
@@ -4268,7 +4260,7 @@
         <v>3840.1899994920041</v>
       </c>
     </row>
-    <row r="100" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F100" s="1">
         <v>95</v>
       </c>
@@ -4304,7 +4296,7 @@
         <v>4068.5396014507974</v>
       </c>
     </row>
-    <row r="101" spans="6:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F101" s="1">
         <v>96</v>
       </c>
@@ -4336,8 +4328,44 @@
         <v>4248.2392811936988</v>
       </c>
       <c r="N101" s="4">
-        <f>AVERAGE(K101,K101*C6)</f>
+        <f t="shared" si="18"/>
         <v>4310.4675786258267</v>
+      </c>
+    </row>
+    <row r="102" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F102" s="1">
+        <v>97</v>
+      </c>
+      <c r="G102" t="s">
+        <v>108</v>
+      </c>
+      <c r="H102" s="4">
+        <f t="shared" ref="H102" si="19">AVERAGE(K101,K102)</f>
+        <v>4310.4675786258267</v>
+      </c>
+      <c r="I102" s="4">
+        <f t="shared" ref="I102" si="20">K102-(K102-H102)*I$3</f>
+        <v>4372.6958760579546</v>
+      </c>
+      <c r="J102" s="4">
+        <f t="shared" ref="J102" si="21">K102-(K102-H102)*J$3</f>
+        <v>4422.4785140036574</v>
+      </c>
+      <c r="K102" s="4">
+        <f t="shared" si="14"/>
+        <v>4434.9241734900834</v>
+      </c>
+      <c r="L102" s="4">
+        <f t="shared" ref="L102" si="22">K102+(N102-K102)*L$3</f>
+        <v>4448.1098904711162</v>
+      </c>
+      <c r="M102" s="4">
+        <f t="shared" ref="M102" si="23">K102+(N102-K102)*M$3</f>
+        <v>4500.8527583952473</v>
+      </c>
+      <c r="N102" s="4">
+        <f>AVERAGE(K102,K102*$C$6)</f>
+        <v>4566.7813433004121</v>
       </c>
     </row>
   </sheetData>
@@ -4349,19 +4377,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAF266D-20C7-46BE-9AC3-78011456380A}">
-  <dimension ref="A4:E100"/>
+  <dimension ref="A4:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="3" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="3" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>15.892724695152365</v>
       </c>
@@ -4378,7 +4406,7 @@
         <v>16.594676210369911</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>16.83775537297268</v>
       </c>
@@ -4395,7 +4423,7 @@
         <v>17.58144710133476</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>17.838980504491296</v>
       </c>
@@ -4412,7 +4440,7 @@
         <v>18.626894448466143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>18.899741586127917</v>
       </c>
@@ -4429,7 +4457,7 @@
         <v>19.73450733574473</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>20.023578810038</v>
       </c>
@@ -4446,7 +4474,7 @@
         <v>20.907982318900856</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>21.214242879177171</v>
       </c>
@@ -4463,7 +4491,7 @@
         <v>22.151235762327889</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>22.475707524925973</v>
       </c>
@@ -4480,7 +4508,7 @@
         <v>23.468416909586772</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>23.812182769051404</v>
       </c>
@@ -4497,7 +4525,7 @@
         <v>24.863921731123227</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>25.228128974265786</v>
       </c>
@@ -4514,7 +4542,7 @@
         <v>26.342407595413185</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>26.728271730275456</v>
       </c>
@@ -4531,7 +4559,7 @@
         <v>27.908808812500002</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>28.317617625000004</v>
       </c>
@@ -4548,7 +4576,7 @@
         <v>29.568353101798571</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>30.001470953597142</v>
       </c>
@@ -4565,7 +4593,7 @@
         <v>31.326579039126138</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>31.785451421057989</v>
       </c>
@@ -4582,7 +4610,7 @@
         <v>33.189354541187598</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>33.675512897453501</v>
       </c>
@@ -4599,7 +4627,7 @@
         <v>35.162896449205697</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>35.677963288426078</v>
       </c>
@@ -4616,7 +4644,7 @@
         <v>37.253791277054461</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>37.799485587242089</v>
       </c>
@@ -4633,7 +4661,7 @@
         <v>39.469017193141084</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>40.047160178664832</v>
       </c>
@@ -4650,7 +4678,7 @@
         <v>41.815967309398559</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>42.428488469084797</v>
       </c>
@@ -4667,7 +4695,7 @@
         <v>44.302474355114057</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>44.95141792177084</v>
       </c>
@@ -4684,7 +4712,7 @@
         <v>46.93683681793965</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>47.624368580794894</v>
       </c>
@@ -4701,7 +4729,7 @@
         <v>49.727846639328483</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>50.456261172151571</v>
       </c>
@@ -4718,7 +4746,7 @@
         <v>52.684818556827537</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>53.456546875857342</v>
       </c>
@@ -4735,7 +4763,7 @@
         <v>55.817621191154039</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>56.635238868391141</v>
       </c>
@@ -4752,7 +4780,7 @@
         <v>59.136709981805751</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>60.002945740746171</v>
       </c>
@@ -4769,7 +4797,7 @@
         <v>62.653162081124876</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>63.570906903622742</v>
       </c>
@@ -4786,7 +4814,7 @@
         <v>66.378713323271015</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>67.351030097923555</v>
       </c>
@@ -4803,7 +4831,7 @@
         <v>70.325797391484031</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>71.355931135739411</v>
       </c>
@@ -4820,7 +4848,7 @@
         <v>74.507587314353586</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>75.598976004457</v>
       </c>
@@ -4837,7 +4865,7 @@
         <v>78.938039429585729</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>80.094325474507627</v>
       </c>
@@ -4854,7 +4882,7 @@
         <v>83.631939961991137</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>84.856982359630834</v>
       </c>
@@ -4871,7 +4899,7 @@
         <v>88.604954371145027</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>89.902841587379811</v>
       </c>
@@ -4888,7 +4916,7 @@
         <v>93.873679633411854</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>95.248743246974328</v>
       </c>
@@ -4905,7 +4933,7 @@
         <v>99.455699632821393</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>100.91252879154351</v>
       </c>
@@ -4922,7 +4950,7 @@
         <v>105.36964384565783</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>106.91310058232794</v>
       </c>
@@ -4939,7 +4967,7 @@
         <v>111.63524951461658</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>113.27048497356498</v>
       </c>
@@ -4956,7 +4984,7 @@
         <v>118.2734275200292</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>120.0058991485966</v>
       </c>
@@ -4973,7 +5001,7 @@
         <v>125.30633216799546</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>127.14182193025952</v>
       </c>
@@ -4990,7 +5018,7 @@
         <v>132.75743512833421</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>134.70206880188076</v>
       </c>
@@ -5007,7 +5035,7 @@
         <v>140.65160376911388</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>142.71187138925387</v>
       </c>
@@ -5024,7 +5052,7 @@
         <v>149.01518414919707</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>151.19796166886024</v>
       </c>
@@ -5041,7 +5069,7 @@
         <v>157.8760889457792</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>160.18866118337186</v>
       </c>
@@ -5058,7 +5086,7 @@
         <v>167.26389061037099</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>169.71397556218483</v>
       </c>
@@ -5075,7 +5103,7 @@
         <v>177.20992006412456</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>179.80569466243662</v>
       </c>
@@ -5092,7 +5120,7 @@
         <v>187.74737126188961</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>190.49749866471853</v>
       </c>
@@ -5109,7 +5137,7 @@
         <v>198.91141197397252</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>201.8250704775686</v>
       </c>
@@ -5126,7 +5154,7 @@
         <v>210.73930115532204</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>213.82621482588331</v>
       </c>
@@ -5143,7 +5171,7 @@
         <v>223.27051329385108</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>226.5409844206963</v>
       </c>
@@ -5160,7 +5188,7 @@
         <v>236.54687015289471</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>240.01181363140267</v>
       </c>
@@ -5177,7 +5205,7 @@
         <v>250.61268034748335</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>254.28366010654815</v>
       </c>
@@ -5194,7 +5222,7 @@
         <v>265.51488722025385</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>269.40415481582988</v>
       </c>
@@ -5211,7 +5239,7 @@
         <v>281.30322551052052</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>285.42376101405904</v>
       </c>
@@ -5228,7 +5256,7 @@
         <v>298.03038733937512</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>302.39594265761417</v>
       </c>
@@ -5245,7 +5273,7 @@
         <v>315.7521980647752</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>320.37734283545819</v>
       </c>
@@ -5262,7 +5290,7 @@
         <v>334.52780259352079</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>339.4279728102174</v>
       </c>
@@ -5279,7 +5307,7 @@
         <v>354.41986277191961</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>359.61141230022861</v>
       </c>
@@ -5296,7 +5324,7 @@
         <v>375.49476651391257</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>380.99502167097842</v>
       </c>
@@ -5313,7 +5341,7 @@
         <v>397.82284936460599</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>403.65016674410197</v>
       </c>
@@ -5330,7 +5358,7 @@
         <v>421.47862923865858</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>427.65245697422324</v>
       </c>
@@ -5347,7 +5375,7 @@
         <v>446.5410551169399</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>453.08199778852725</v>
       </c>
@@ -5364,7 +5392,7 @@
         <v>473.09377053146409</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>480.02365793122624</v>
       </c>
@@ -5381,7 +5409,7 @@
         <v>501.22539271795364</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>508.56735270515662</v>
       </c>
@@ -5398,7 +5426,7 @@
         <v>531.02980836768063</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>538.80834405579867</v>
       </c>
@@ -5415,7 +5443,7 @@
         <v>562.60648696562896</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>570.84755849922317</v>
       </c>
@@ -5432,7 +5460,7 @@
         <v>596.06081276071495</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>604.79192395501832</v>
       </c>
@@ -5449,7 +5477,7 @@
         <v>631.50443647598649</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>640.75472660834794</v>
       </c>
@@ -5466,7 +5494,7 @@
         <v>669.05564793260191</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>678.85598899213289</v>
       </c>
@@ -5483,7 +5511,7 @@
         <v>708.83977083118305</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>719.22287055117113</v>
       </c>
@@ -5500,7 +5528,7 @@
         <v>750.98958100809477</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>761.99009202504249</v>
       </c>
@@ -5517,7 +5545,7 @@
         <v>795.64574956253728</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>807.30038506613687</v>
       </c>
@@ -5534,7 +5562,7 @@
         <v>842.95731233334959</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>855.30496859336313</v>
       </c>
@@ -5551,7 +5579,7 @@
         <v>893.08216729235892</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>906.16405347132729</v>
       </c>
@@ -5568,7 +5596,7 @@
         <v>946.18760151428114</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>960.04737719929824</v>
       </c>
@@ -5585,7 +5613,7 @@
         <v>1002.4508494818851</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>1017.1347703944379</v>
       </c>
@@ -5602,7 +5630,7 @@
         <v>1062.0596845897112</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>1077.6167569598792</v>
       </c>
@@ -5619,7 +5647,7 @@
         <v>1125.2130458204379</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>1141.6951899406604</v>
       </c>
@@ -5636,7 +5664,7 @@
         <v>1192.1217016853632</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>1209.5839251896209</v>
       </c>
@@ -5653,7 +5681,7 @@
         <v>1263.0089536448502</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>1281.509535091564</v>
       </c>
@@ -5670,7 +5698,7 @@
         <v>1338.1113813563295</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>1357.7120647276674</v>
       </c>
@@ -5687,7 +5715,7 @@
         <v>1417.6796322370592</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>1438.4458330037751</v>
       </c>
@@ -5704,7 +5732,7 @@
         <v>1501.9792579767347</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>1523.9802814162622</v>
       </c>
@@ -5721,7 +5749,7 @@
         <v>1591.2916007917311</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>1614.6008732881455</v>
       </c>
@@ -5738,7 +5766,7 @@
         <v>1685.9147323787702</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>1710.6100464765659</v>
       </c>
@@ -5755,7 +5783,7 @@
         <v>1786.1644487016824</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>1812.328222731207</v>
       </c>
@@ -5772,7 +5800,7 @@
         <v>1892.3753239312755</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>1920.094877072295</v>
       </c>
@@ -5789,7 +5817,7 @@
         <v>2004.9018270557335</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>2034.2696707571326</v>
       </c>
@@ -5806,7 +5834,7 @@
         <v>2124.1195048881314</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>2155.2336516163314</v>
       </c>
@@ -5823,7 +5851,7 @@
         <v>2250.4262354192451</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>2283.3905257657589</v>
       </c>
@@ -5840,7 +5868,7 @@
         <v>2384.2435556986029</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>2419.1680049384204</v>
       </c>
@@ -5857,7 +5885,7 @@
         <v>2526.0180686754647</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>2563.0192339328746</v>
       </c>
@@ -5874,7 +5902,7 @@
         <v>2676.2229336949213</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>2715.4243029421486</v>
       </c>
@@ -5891,7 +5919,7 @@
         <v>2835.359445623516</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>2876.8918498104285</v>
       </c>
@@ -5908,7 +5936,7 @@
         <v>3003.9587078745726</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>3047.9607575648915</v>
       </c>
@@ -5925,7 +5953,7 @@
         <v>3182.5834049167888</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>3229.2019528880483</v>
       </c>
@@ -5942,7 +5970,7 @@
         <v>3371.8296801816969</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>3421.2203115328261</v>
       </c>
@@ -5959,7 +5987,7 @@
         <v>3572.3291256373095</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>3624.6566770395339</v>
       </c>
@@ -5976,7 +6004,7 @@
         <v>3784.7508896679938</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>3840.1899994920041</v>
       </c>
@@ -5993,7 +6021,7 @@
         <v>4009.8039102954108</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>4068.5396014507974</v>
       </c>
@@ -6008,6 +6036,23 @@
       </c>
       <c r="E100" s="8">
         <v>4248.2392811936988</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="8">
+        <v>4310.4675786258267</v>
+      </c>
+      <c r="B101" s="8">
+        <v>4372.6958760579546</v>
+      </c>
+      <c r="C101" s="8">
+        <v>4422.4785140036574</v>
+      </c>
+      <c r="D101" s="8">
+        <v>4448.1098904711162</v>
+      </c>
+      <c r="E101" s="8">
+        <v>4500.8527583952473</v>
       </c>
     </row>
   </sheetData>
@@ -6017,16 +6062,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD18E7B-735D-4773-BB44-4B2F2D1D3EBC}">
-  <dimension ref="B1:F97"/>
+  <dimension ref="B1:F98"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98:F98"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="7">
         <v>15.892724695152365</v>
       </c>
@@ -6043,7 +6090,7 @@
         <v>16.594676210369911</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7">
         <v>16.83775537297268</v>
       </c>
@@ -6060,7 +6107,7 @@
         <v>17.58144710133476</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>17.838980504491296</v>
       </c>
@@ -6077,7 +6124,7 @@
         <v>18.626894448466143</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>18.899741586127917</v>
       </c>
@@ -6094,7 +6141,7 @@
         <v>19.73450733574473</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>20.023578810038</v>
       </c>
@@ -6111,7 +6158,7 @@
         <v>20.907982318900856</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>21.214242879177171</v>
       </c>
@@ -6128,7 +6175,7 @@
         <v>22.151235762327889</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>22.475707524925973</v>
       </c>
@@ -6145,7 +6192,7 @@
         <v>23.468416909586772</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>23.812182769051404</v>
       </c>
@@ -6162,7 +6209,7 @@
         <v>24.863921731123227</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>25.228128974265786</v>
       </c>
@@ -6179,7 +6226,7 @@
         <v>26.342407595413185</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>26.728271730275456</v>
       </c>
@@ -6196,7 +6243,7 @@
         <v>27.908808812500002</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>28.317617625000004</v>
       </c>
@@ -6213,7 +6260,7 @@
         <v>29.568353101798571</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>30.001470953597142</v>
       </c>
@@ -6230,7 +6277,7 @@
         <v>31.326579039126138</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>31.785451421057989</v>
       </c>
@@ -6247,7 +6294,7 @@
         <v>33.189354541187598</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>33.675512897453501</v>
       </c>
@@ -6264,7 +6311,7 @@
         <v>35.162896449205697</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>35.677963288426078</v>
       </c>
@@ -6281,7 +6328,7 @@
         <v>37.253791277054461</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>37.799485587242089</v>
       </c>
@@ -6298,7 +6345,7 @@
         <v>39.469017193141084</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>40.047160178664832</v>
       </c>
@@ -6315,7 +6362,7 @@
         <v>41.815967309398559</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>42.428488469084797</v>
       </c>
@@ -6332,7 +6379,7 @@
         <v>44.302474355114057</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>44.95141792177084</v>
       </c>
@@ -6349,7 +6396,7 @@
         <v>46.93683681793965</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>47.624368580794894</v>
       </c>
@@ -6366,7 +6413,7 @@
         <v>49.727846639328483</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>50.456261172151571</v>
       </c>
@@ -6383,7 +6430,7 @@
         <v>52.684818556827537</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>53.456546875857342</v>
       </c>
@@ -6400,7 +6447,7 @@
         <v>55.817621191154039</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>56.635238868391141</v>
       </c>
@@ -6417,7 +6464,7 @@
         <v>59.136709981805751</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>60.002945740746171</v>
       </c>
@@ -6434,7 +6481,7 @@
         <v>62.653162081124876</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>63.570906903622742</v>
       </c>
@@ -6451,7 +6498,7 @@
         <v>66.378713323271015</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>67.351030097923555</v>
       </c>
@@ -6468,7 +6515,7 @@
         <v>70.325797391484031</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>71.355931135739411</v>
       </c>
@@ -6485,7 +6532,7 @@
         <v>74.507587314353586</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <v>75.598976004457</v>
       </c>
@@ -6502,7 +6549,7 @@
         <v>78.938039429585729</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <v>80.094325474507627</v>
       </c>
@@ -6519,7 +6566,7 @@
         <v>83.631939961991137</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <v>84.856982359630834</v>
       </c>
@@ -6536,7 +6583,7 @@
         <v>88.604954371145027</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="7">
         <v>89.902841587379811</v>
       </c>
@@ -6553,7 +6600,7 @@
         <v>93.873679633411854</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="7">
         <v>95.248743246974328</v>
       </c>
@@ -6570,7 +6617,7 @@
         <v>99.455699632821393</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="7">
         <v>100.91252879154351</v>
       </c>
@@ -6587,7 +6634,7 @@
         <v>105.36964384565783</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="7">
         <v>106.91310058232794</v>
       </c>
@@ -6604,7 +6651,7 @@
         <v>111.63524951461658</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="7">
         <v>113.27048497356498</v>
       </c>
@@ -6621,7 +6668,7 @@
         <v>118.2734275200292</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="7">
         <v>120.0058991485966</v>
       </c>
@@ -6638,7 +6685,7 @@
         <v>125.30633216799546</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="7">
         <v>127.14182193025952</v>
       </c>
@@ -6655,7 +6702,7 @@
         <v>132.75743512833421</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="7">
         <v>134.70206880188076</v>
       </c>
@@ -6672,7 +6719,7 @@
         <v>140.65160376911388</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="7">
         <v>142.71187138925387</v>
       </c>
@@ -6689,7 +6736,7 @@
         <v>149.01518414919707</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="7">
         <v>151.19796166886024</v>
       </c>
@@ -6706,7 +6753,7 @@
         <v>157.8760889457792</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
         <v>160.18866118337186</v>
       </c>
@@ -6723,7 +6770,7 @@
         <v>167.26389061037099</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
         <v>169.71397556218483</v>
       </c>
@@ -6740,7 +6787,7 @@
         <v>177.20992006412456</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="7">
         <v>179.80569466243662</v>
       </c>
@@ -6757,7 +6804,7 @@
         <v>187.74737126188961</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
         <v>190.49749866471853</v>
       </c>
@@ -6774,7 +6821,7 @@
         <v>198.91141197397252</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="7">
         <v>201.8250704775686</v>
       </c>
@@ -6791,7 +6838,7 @@
         <v>210.73930115532204</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="7">
         <v>213.82621482588331</v>
       </c>
@@ -6808,7 +6855,7 @@
         <v>223.27051329385108</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
         <v>226.5409844206963</v>
       </c>
@@ -6825,7 +6872,7 @@
         <v>236.54687015289471</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
         <v>240.01181363140267</v>
       </c>
@@ -6842,7 +6889,7 @@
         <v>250.61268034748335</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
         <v>254.28366010654815</v>
       </c>
@@ -6859,7 +6906,7 @@
         <v>265.51488722025385</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
         <v>269.40415481582988</v>
       </c>
@@ -6876,7 +6923,7 @@
         <v>281.30322551052052</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
         <v>285.42376101405904</v>
       </c>
@@ -6893,7 +6940,7 @@
         <v>298.03038733937512</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>302.39594265761417</v>
       </c>
@@ -6910,7 +6957,7 @@
         <v>315.7521980647752</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="7">
         <v>320.37734283545819</v>
       </c>
@@ -6927,7 +6974,7 @@
         <v>334.52780259352079</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
         <v>339.4279728102174</v>
       </c>
@@ -6944,7 +6991,7 @@
         <v>354.41986277191961</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="7">
         <v>359.61141230022861</v>
       </c>
@@ -6961,7 +7008,7 @@
         <v>375.49476651391257</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
         <v>380.99502167097842</v>
       </c>
@@ -6978,7 +7025,7 @@
         <v>397.82284936460599</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="7">
         <v>403.65016674410197</v>
       </c>
@@ -6995,7 +7042,7 @@
         <v>421.47862923865858</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
         <v>427.65245697422324</v>
       </c>
@@ -7012,7 +7059,7 @@
         <v>446.5410551169399</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="7">
         <v>453.08199778852725</v>
       </c>
@@ -7029,7 +7076,7 @@
         <v>473.09377053146409</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
         <v>480.02365793122624</v>
       </c>
@@ -7046,7 +7093,7 @@
         <v>501.22539271795364</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="7">
         <v>508.56735270515662</v>
       </c>
@@ -7063,7 +7110,7 @@
         <v>531.02980836768063</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
         <v>538.80834405579867</v>
       </c>
@@ -7080,7 +7127,7 @@
         <v>562.60648696562896</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="7">
         <v>570.84755849922317</v>
       </c>
@@ -7097,7 +7144,7 @@
         <v>596.06081276071495</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="7">
         <v>604.79192395501832</v>
       </c>
@@ -7114,7 +7161,7 @@
         <v>631.50443647598649</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="7">
         <v>640.75472660834794</v>
       </c>
@@ -7131,7 +7178,7 @@
         <v>669.05564793260191</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="7">
         <v>678.85598899213289</v>
       </c>
@@ -7148,7 +7195,7 @@
         <v>708.83977083118305</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="7">
         <v>719.22287055117113</v>
       </c>
@@ -7165,7 +7212,7 @@
         <v>750.98958100809477</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
         <v>761.99009202504249</v>
       </c>
@@ -7182,7 +7229,7 @@
         <v>795.64574956253728</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="7">
         <v>807.30038506613687</v>
       </c>
@@ -7199,7 +7246,7 @@
         <v>842.95731233334959</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
         <v>855.30496859336313</v>
       </c>
@@ -7216,7 +7263,7 @@
         <v>893.08216729235892</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="7">
         <v>906.16405347132729</v>
       </c>
@@ -7233,7 +7280,7 @@
         <v>946.18760151428114</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
         <v>960.04737719929824</v>
       </c>
@@ -7250,7 +7297,7 @@
         <v>1002.4508494818851</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="7">
         <v>1017.1347703944379</v>
       </c>
@@ -7267,7 +7314,7 @@
         <v>1062.0596845897112</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="7">
         <v>1077.6167569598792</v>
       </c>
@@ -7284,7 +7331,7 @@
         <v>1125.2130458204379</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="7">
         <v>1141.6951899406604</v>
       </c>
@@ -7301,7 +7348,7 @@
         <v>1192.1217016853632</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
         <v>1209.5839251896209</v>
       </c>
@@ -7318,7 +7365,7 @@
         <v>1263.0089536448502</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="7">
         <v>1281.509535091564</v>
       </c>
@@ -7335,7 +7382,7 @@
         <v>1338.1113813563295</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
         <v>1357.7120647276674</v>
       </c>
@@ -7352,7 +7399,7 @@
         <v>1417.6796322370592</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="7">
         <v>1438.4458330037751</v>
       </c>
@@ -7369,7 +7416,7 @@
         <v>1501.9792579767347</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
         <v>1523.9802814162622</v>
       </c>
@@ -7386,7 +7433,7 @@
         <v>1591.2916007917311</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="7">
         <v>1614.6008732881455</v>
       </c>
@@ -7403,7 +7450,7 @@
         <v>1685.9147323787702</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="7">
         <v>1710.6100464765659</v>
       </c>
@@ -7420,7 +7467,7 @@
         <v>1786.1644487016824</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="7">
         <v>1812.328222731207</v>
       </c>
@@ -7437,7 +7484,7 @@
         <v>1892.3753239312755</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
         <v>1920.094877072295</v>
       </c>
@@ -7454,7 +7501,7 @@
         <v>2004.9018270557335</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="7">
         <v>2034.2696707571326</v>
       </c>
@@ -7471,7 +7518,7 @@
         <v>2124.1195048881314</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="7">
         <v>2155.2336516163314</v>
       </c>
@@ -7488,7 +7535,7 @@
         <v>2250.4262354192451</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="7">
         <v>2283.3905257657589</v>
       </c>
@@ -7505,7 +7552,7 @@
         <v>2384.2435556986029</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="7">
         <v>2419.1680049384204</v>
       </c>
@@ -7522,7 +7569,7 @@
         <v>2526.0180686754647</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="7">
         <v>2563.0192339328746</v>
       </c>
@@ -7539,7 +7586,7 @@
         <v>2676.2229336949213</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="7">
         <v>2715.4243029421486</v>
       </c>
@@ -7556,7 +7603,7 @@
         <v>2835.359445623516</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="7">
         <v>2876.8918498104285</v>
       </c>
@@ -7573,7 +7620,7 @@
         <v>3003.9587078745726</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="7">
         <v>3047.9607575648915</v>
       </c>
@@ -7590,7 +7637,7 @@
         <v>3182.5834049167888</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="7">
         <v>3229.2019528880483</v>
       </c>
@@ -7607,7 +7654,7 @@
         <v>3371.8296801816969</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="7">
         <v>3421.2203115328261</v>
       </c>
@@ -7624,7 +7671,7 @@
         <v>3572.3291256373095</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="7">
         <v>3624.6566770395339</v>
       </c>
@@ -7641,7 +7688,7 @@
         <v>3784.7508896679938</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="7">
         <v>3840.1899994920041</v>
       </c>
@@ -7658,7 +7705,7 @@
         <v>4009.8039102954108</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="7">
         <v>4068.5396014507974</v>
       </c>
@@ -7673,6 +7720,23 @@
       </c>
       <c r="F97" s="7">
         <v>4248.2392811936988</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="7">
+        <v>4310.4675786258267</v>
+      </c>
+      <c r="C98" s="7">
+        <v>4372.6958760579546</v>
+      </c>
+      <c r="D98" s="7">
+        <v>4422.4785140036574</v>
+      </c>
+      <c r="E98" s="7">
+        <v>4448.1098904711162</v>
+      </c>
+      <c r="F98" s="7">
+        <v>4500.8527583952473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>